<commit_message>
Added assets and added button disabling
</commit_message>
<xml_diff>
--- a/static/game_scoring/Game_Scoring.xlsx
+++ b/static/game_scoring/Game_Scoring.xlsx
@@ -188,8 +188,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFBFD7FE"/>
-        <bgColor rgb="FFBFD7FE"/>
+        <fgColor rgb="FF92B9F7"/>
+        <bgColor rgb="FF92B9F7"/>
       </patternFill>
     </fill>
     <fill>
@@ -200,26 +200,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFA3"/>
-        <bgColor rgb="FFFFFFA3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCACA"/>
-        <bgColor rgb="FFFFCACA"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFABAB"/>
-        <bgColor rgb="FFFFABAB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE5BDFF"/>
-        <bgColor rgb="FFE5BDFF"/>
+        <fgColor rgb="FFE5E593"/>
+        <bgColor rgb="FFE5E593"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE59393"/>
+        <bgColor rgb="FFE59393"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9900FF"/>
+        <bgColor rgb="FF9900FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -290,10 +290,10 @@
     <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="14" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="15" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="14" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="15" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="16" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">

</xml_diff>